<commit_message>
final additions portfolio 1
</commit_message>
<xml_diff>
--- a/Old.xlsx
+++ b/Old.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elaynaseago/Downloads/R_Class/portfolio-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{353DBB38-A1CE-164F-8BBF-1B5F5FD32154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1E0743-7149-554B-BA48-16B4BA35D3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" xr2:uid="{7C5EBFE9-C1B6-CC43-961D-F1A93D96713B}"/>
+    <workbookView xWindow="2060" yWindow="600" windowWidth="25600" windowHeight="14540" xr2:uid="{7C5EBFE9-C1B6-CC43-961D-F1A93D96713B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEE2639-6DCB-CD4E-A675-E21853FD1F60}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,7 +440,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>960.14</v>
+        <v>1124.3317799690401</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>671.49</v>
+        <v>1709.4064235687301</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1040.52</v>
+        <v>1161.0686566148499</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -485,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>794.9</v>
+        <v>1265.55928346273</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>900.95</v>
+        <v>1371.3963761049199</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -515,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>618.04999999999995</v>
+        <v>1042.64877856463</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -530,7 +530,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>678.22</v>
+        <v>1158.8322371244399</v>
       </c>
       <c r="H8" s="3"/>
     </row>
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>954.63</v>
+        <v>1433.06936614815</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -560,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1074.82</v>
+        <v>960.36616037058297</v>
       </c>
       <c r="H10" s="3"/>
     </row>
@@ -575,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1073.44</v>
+        <v>1033.8311251472001</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -590,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>1068.4000000000001</v>
+        <v>935.57915299437798</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -605,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1000.83</v>
+        <v>1210.5998289890799</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>830.64</v>
+        <v>1135.0335563932099</v>
       </c>
       <c r="H14" s="3"/>
     </row>
@@ -635,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>865.02</v>
+        <v>1264.2417308446502</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>1087.3800000000001</v>
+        <v>754.35857150865604</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -665,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>936.39</v>
+        <v>1120.8502159842999</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -680,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>1026.49</v>
+        <v>1159.7366174062101</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -695,43 +695,43 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>746.41</v>
+        <v>1029.3267165913301</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>785.05</v>
+        <v>1665.0309345938902</v>
       </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>1028.42</v>
+        <v>2136.7008459000399</v>
       </c>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -740,13 +740,13 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <v>1120.96</v>
+        <v>1327.8797183718</v>
       </c>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -755,13 +755,13 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>1119.42</v>
+        <v>1433.0873272635699</v>
       </c>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -770,13 +770,13 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>1134.96</v>
+        <v>1573.03722151395</v>
       </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -785,12 +785,12 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <v>1076.74</v>
+        <v>1345.48615587169</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -799,12 +799,12 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>1161.1099999999999</v>
+        <v>1236.48009981428</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -813,12 +813,12 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>843.8</v>
+        <v>1612.12934296707</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -827,12 +827,12 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <v>1056.69</v>
+        <v>1245.8357192851902</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -841,13 +841,13 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>1104.56</v>
+        <v>1106.1112551853601</v>
       </c>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -856,13 +856,13 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>1368.12</v>
+        <v>1201.21844325747</v>
       </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -871,12 +871,12 @@
         <v>2</v>
       </c>
       <c r="D31">
-        <v>1292.72</v>
+        <v>1725.1582336425799</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -885,12 +885,12 @@
         <v>2</v>
       </c>
       <c r="D32">
-        <v>1242.8399999999999</v>
+        <v>1372.63625243614</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -899,12 +899,12 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <v>1206.5</v>
+        <v>1530.34167819553</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -913,12 +913,12 @@
         <v>2</v>
       </c>
       <c r="D34">
-        <v>1140.68</v>
+        <v>685.24928887685098</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -927,12 +927,12 @@
         <v>2</v>
       </c>
       <c r="D35">
-        <v>1250.54</v>
+        <v>1333.3773314952898</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -941,12 +941,12 @@
         <v>2</v>
       </c>
       <c r="D36">
-        <v>1255.31</v>
+        <v>1450.24352807265</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -955,68 +955,68 @@
         <v>2</v>
       </c>
       <c r="D37">
-        <v>1200.07</v>
+        <v>1407.22207839672</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>1276.6500000000001</v>
+        <v>1023.94280066857</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39">
-        <v>1072.4100000000001</v>
+        <v>1850.7387439409899</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>988.36</v>
+        <v>1106.6575050353999</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>1286.72</v>
+        <v>1120.3937941584099</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -1025,12 +1025,12 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <v>1102.97</v>
+        <v>1833.87985935918</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -1039,12 +1039,12 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <v>707.79</v>
+        <v>1326.0178389372602</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -1053,12 +1053,12 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <v>1033.6400000000001</v>
+        <v>1581.7374897003201</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -1067,12 +1067,12 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <v>884.42</v>
+        <v>1504.7991364090501</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -1081,12 +1081,12 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>957.32</v>
+        <v>1159.73693446109</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -1095,12 +1095,12 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <v>743.68</v>
+        <v>1070.7938212614799</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -1109,12 +1109,12 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <v>766.07</v>
+        <v>1043.1753931374399</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -1123,12 +1123,12 @@
         <v>1</v>
       </c>
       <c r="D49">
-        <v>1170.7</v>
+        <v>1063.3954451634299</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -1137,12 +1137,12 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <v>1181.3599999999999</v>
+        <v>1096.77877097294</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -1151,12 +1151,12 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <v>1222.53</v>
+        <v>1225.0432751395499</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -1165,12 +1165,12 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>1101.8599999999999</v>
+        <v>728.25842745163902</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -1179,12 +1179,12 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>1024.1099999999999</v>
+        <v>1312.1229895838999</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -1193,12 +1193,12 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <v>898.36</v>
+        <v>1055.4949097011399</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -1207,96 +1207,96 @@
         <v>1</v>
       </c>
       <c r="D55">
-        <v>909.06</v>
+        <v>1072.96654030129</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B56">
         <v>2</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56">
-        <v>1268.75</v>
+        <v>1052.0749281753199</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B57">
         <v>2</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D57">
-        <v>1062.78</v>
+        <v>1911.1829429864899</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B58">
         <v>2</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D58">
-        <v>1030.06</v>
+        <v>1293.1088268756901</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B59">
         <v>2</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59">
-        <v>952.53</v>
+        <v>1210.82695420966</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B60">
         <v>2</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60">
-        <v>844.18</v>
+        <v>1631.0264943521199</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B61">
         <v>2</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61">
-        <v>1138.25</v>
+        <v>1388.98379007975</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -1305,12 +1305,12 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <v>1080.96</v>
+        <v>1204.1195660829501</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -1319,12 +1319,12 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <v>877.84</v>
+        <v>1554.3478050015201</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -1333,12 +1333,12 @@
         <v>2</v>
       </c>
       <c r="D64">
-        <v>1000.4</v>
+        <v>1107.4298948481501</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -1347,12 +1347,12 @@
         <v>2</v>
       </c>
       <c r="D65">
-        <v>897.93</v>
+        <v>1141.0817476836098</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B66">
         <v>2</v>
@@ -1361,12 +1361,12 @@
         <v>2</v>
       </c>
       <c r="D66">
-        <v>1008.6</v>
+        <v>1194.0285346087301</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -1375,12 +1375,12 @@
         <v>2</v>
       </c>
       <c r="D67">
-        <v>728.02</v>
+        <v>1202.65987442761</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -1389,12 +1389,12 @@
         <v>2</v>
       </c>
       <c r="D68">
-        <v>970.6</v>
+        <v>1128.48304347558</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B69">
         <v>2</v>
@@ -1403,12 +1403,12 @@
         <v>2</v>
       </c>
       <c r="D69">
-        <v>1048.4100000000001</v>
+        <v>1409.6306280656302</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B70">
         <v>2</v>
@@ -1417,12 +1417,12 @@
         <v>2</v>
       </c>
       <c r="D70">
-        <v>1272.48</v>
+        <v>869.45148876735107</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B71">
         <v>2</v>
@@ -1431,12 +1431,12 @@
         <v>2</v>
       </c>
       <c r="D71">
-        <v>1185.94</v>
+        <v>1290.6524151563601</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -1445,12 +1445,12 @@
         <v>2</v>
       </c>
       <c r="D72">
-        <v>1168.99</v>
+        <v>1476.33555688356</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B73">
         <v>2</v>
@@ -1459,119 +1459,7 @@
         <v>2</v>
       </c>
       <c r="D73">
-        <v>1132.4100000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>13</v>
-      </c>
-      <c r="B74">
-        <v>2</v>
-      </c>
-      <c r="C74">
-        <v>2</v>
-      </c>
-      <c r="D74">
-        <v>1055.6300000000001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>14</v>
-      </c>
-      <c r="B75">
-        <v>2</v>
-      </c>
-      <c r="C75">
-        <v>2</v>
-      </c>
-      <c r="D75">
-        <v>1099.1199999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>15</v>
-      </c>
-      <c r="B76">
-        <v>2</v>
-      </c>
-      <c r="C76">
-        <v>2</v>
-      </c>
-      <c r="D76">
-        <v>1164.69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>16</v>
-      </c>
-      <c r="B77">
-        <v>2</v>
-      </c>
-      <c r="C77">
-        <v>2</v>
-      </c>
-      <c r="D77">
-        <v>1008.28</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>17</v>
-      </c>
-      <c r="B78">
-        <v>2</v>
-      </c>
-      <c r="C78">
-        <v>2</v>
-      </c>
-      <c r="D78">
-        <v>1278.32</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>18</v>
-      </c>
-      <c r="B79">
-        <v>2</v>
-      </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
-      <c r="D79">
-        <v>991.8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>19</v>
-      </c>
-      <c r="B80">
-        <v>2</v>
-      </c>
-      <c r="C80">
-        <v>2</v>
-      </c>
-      <c r="D80">
-        <v>838.63</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>20</v>
-      </c>
-      <c r="B81">
-        <v>2</v>
-      </c>
-      <c r="C81">
-        <v>2</v>
-      </c>
-      <c r="D81">
-        <v>1185.6500000000001</v>
+        <v>1214.2383618788299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>